<commit_message>
Inital draft of writeup
</commit_message>
<xml_diff>
--- a/sheets/MyAllGather.xlsx
+++ b/sheets/MyAllGather.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,6 +63,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,15 +101,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -364,11 +384,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1917229280"/>
-        <c:axId val="1917404672"/>
+        <c:axId val="863779440"/>
+        <c:axId val="863783536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1917229280"/>
+        <c:axId val="863779440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,12 +500,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1917404672"/>
+        <c:crossAx val="863783536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1917404672"/>
+        <c:axId val="863783536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,7 +617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1917229280"/>
+        <c:crossAx val="863779440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -936,11 +956,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1947499856"/>
-        <c:axId val="1947502976"/>
+        <c:axId val="863812288"/>
+        <c:axId val="863816048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1947499856"/>
+        <c:axId val="863812288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1052,12 +1072,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1947502976"/>
+        <c:crossAx val="863816048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1947502976"/>
+        <c:axId val="863816048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,7 +1189,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1947499856"/>
+        <c:crossAx val="863812288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1508,11 +1528,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1915688832"/>
-        <c:axId val="1915470640"/>
+        <c:axId val="863841856"/>
+        <c:axId val="863845616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1915688832"/>
+        <c:axId val="863841856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1624,12 +1644,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1915470640"/>
+        <c:crossAx val="863845616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1915470640"/>
+        <c:axId val="863845616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,7 +1761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1915688832"/>
+        <c:crossAx val="863841856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2080,11 +2100,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1949609968"/>
-        <c:axId val="1949612096"/>
+        <c:axId val="863871424"/>
+        <c:axId val="863875184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1949609968"/>
+        <c:axId val="863871424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,12 +2216,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1949612096"/>
+        <c:crossAx val="863875184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1949612096"/>
+        <c:axId val="863875184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2313,7 +2333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1949609968"/>
+        <c:crossAx val="863871424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2652,11 +2672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1916807280"/>
-        <c:axId val="1917184272"/>
+        <c:axId val="863904032"/>
+        <c:axId val="863907792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1916807280"/>
+        <c:axId val="863904032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2768,12 +2788,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1917184272"/>
+        <c:crossAx val="863907792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1917184272"/>
+        <c:axId val="863907792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2885,7 +2905,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916807280"/>
+        <c:crossAx val="863904032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3224,11 +3244,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1948895648"/>
-        <c:axId val="1948898080"/>
+        <c:axId val="863937168"/>
+        <c:axId val="863940928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1948895648"/>
+        <c:axId val="863937168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3340,12 +3360,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1948898080"/>
+        <c:crossAx val="863940928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1948898080"/>
+        <c:axId val="863940928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3457,7 +3477,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1948895648"/>
+        <c:crossAx val="863937168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3796,11 +3816,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1949697488"/>
-        <c:axId val="1950115536"/>
+        <c:axId val="863966736"/>
+        <c:axId val="863970496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1949697488"/>
+        <c:axId val="863966736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3912,12 +3932,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1950115536"/>
+        <c:crossAx val="863970496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1950115536"/>
+        <c:axId val="863970496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4029,7 +4049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1949697488"/>
+        <c:crossAx val="863966736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8007,13 +8027,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>317500</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -8036,16 +8056,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8069,15 +8089,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8100,16 +8120,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8132,16 +8152,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8165,15 +8185,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8196,16 +8216,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8494,8 +8514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O61" sqref="O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9222,6 +9242,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>